<commit_message>
UI: - corrected minus label
API Connection:
- corrected weather ID
</commit_message>
<xml_diff>
--- a/WeatherIDs.xlsx
+++ b/WeatherIDs.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Weather IDs</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>10d</t>
+  </si>
+  <si>
+    <t>Moderate Rain</t>
   </si>
 </sst>
 </file>
@@ -204,13 +207,13 @@
   </cellStyles>
   <dxfs count="6">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -264,12 +267,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Aufgaben" displayName="Aufgaben" ref="B6:D11" totalsRowShown="0">
-  <autoFilter ref="B6:D11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Aufgaben" displayName="Aufgaben" ref="B6:D12" totalsRowShown="0">
+  <autoFilter ref="B6:D12"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="ID" dataDxfId="0"/>
+    <tableColumn id="1" name="ID" dataDxfId="2"/>
     <tableColumn id="2" name="Name" dataDxfId="1"/>
-    <tableColumn id="3" name="IconID" dataDxfId="2"/>
+    <tableColumn id="3" name="IconID" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Aufgaben" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -550,7 +553,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -654,7 +657,13 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B12" s="15"/>
+      <c r="B12" s="16">
+        <v>501</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="18"/>
     </row>
     <row r="13" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="15"/>

</xml_diff>